<commit_message>
Fixed removal estimates, added tutorial to vignette
</commit_message>
<xml_diff>
--- a/Tutorial/TransectsDistanceTutorial.xlsx
+++ b/Tutorial/TransectsDistanceTutorial.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Primary observer (double observer survey)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary observer (double observer survey)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transect length (if transect survey)</t>
+    <t xml:space="preserve">Primary observer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary observer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transect length </t>
   </si>
   <si>
     <t xml:space="preserve">Transect number</t>
@@ -150,7 +150,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>